<commit_message>
07.06 - Rezultate, experiment 1
</commit_message>
<xml_diff>
--- a/Documentatie/RezultateExperimentale/W4W5_BeliuGroseniIneu_01_06.xlsx
+++ b/Documentatie/RezultateExperimentale/W4W5_BeliuGroseniIneu_01_06.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="W4W5_BeliuGroseniIneu_01_06" sheetId="1" r:id="rId1"/>
@@ -1647,24 +1647,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="142090240"/>
-        <c:axId val="142091776"/>
+        <c:axId val="87510016"/>
+        <c:axId val="87581440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142090240"/>
+        <c:axId val="87510016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142091776"/>
+        <c:crossAx val="87581440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142091776"/>
+        <c:axId val="87581440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1672,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142090240"/>
+        <c:crossAx val="87510016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1685,7 +1685,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2674,24 +2674,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="142128256"/>
-        <c:axId val="142129792"/>
+        <c:axId val="87723392"/>
+        <c:axId val="87943040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142128256"/>
+        <c:axId val="87723392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142129792"/>
+        <c:crossAx val="87943040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142129792"/>
+        <c:axId val="87943040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2699,7 +2699,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142128256"/>
+        <c:crossAx val="87723392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2712,7 +2712,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3701,24 +3701,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="142153984"/>
-        <c:axId val="142163968"/>
+        <c:axId val="88013056"/>
+        <c:axId val="88031232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142153984"/>
+        <c:axId val="88013056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="t"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142163968"/>
+        <c:crossAx val="88031232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142163968"/>
+        <c:axId val="88031232"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3726,7 +3726,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142153984"/>
+        <c:crossAx val="88013056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3739,7 +3739,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4728,24 +4728,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="142175616"/>
-        <c:axId val="142197888"/>
+        <c:axId val="88085248"/>
+        <c:axId val="88086784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142175616"/>
+        <c:axId val="88085248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142197888"/>
+        <c:crossAx val="88086784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142197888"/>
+        <c:axId val="88086784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4753,7 +4753,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142175616"/>
+        <c:crossAx val="88085248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4766,7 +4766,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4788,6 +4788,1033 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>W4W5_BeliuGroseniIneu_01_06!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>O3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>W4W5_BeliuGroseniIneu_01_06!$B$2:$B$159</c:f>
+              <c:strCache>
+                <c:ptCount val="156"/>
+                <c:pt idx="0">
+                  <c:v>1/6/2020  3:52:57 AM -Intrat padure</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1/6/2020 4:09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1/6/2020 4:10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1/6/2020 4:11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1/6/2020 4:12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1/6/2020 4:13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1/6/2020 4:14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1/6/2020 4:15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1/6/2020 4:16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1/6/2020 4:17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1/6/2020 4:18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1/6/2020 4:19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1/6/2020  4:20:11 AM - Plecat SatVacanta</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1/6/2020 4:21</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1/6/2020 4:22</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1/6/2020 4:23</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1/6/2020  4:24:15 AM - Iesit Padure</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1/6/2020 4:25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1/6/2020 4:26</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1/6/2020 4:27</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1/6/2020 4:28</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1/6/2020 4:29</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1/6/2020  4:30:22 AM - Barzesti</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1/6/2020 4:33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1/6/2020 4:34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1/6/2020 4:35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1/6/2020 4:36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1/6/2020 4:37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1/6/2020 4:38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1/6/2020 4:39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1/6/2020 4:40</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1/6/2020 4:41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1/6/2020 4:42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1/6/2020 4:43</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1/6/2020 4:44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1/6/2020 4:45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1/6/2020 4:46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1/6/2020 4:47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1/6/2020 4:48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1/6/2020 4:50</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1/6/2020 4:52</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1/6/2020 4:53</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1/6/2020 4:54</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1/6/2020 4:55</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1/6/2020 4:56</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1/6/2020 4:57</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1/6/2020 4:58</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1/6/2020 4:59</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1/6/2020  5:00:16 AM - Intrare Beliu</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1/6/2020 5:01</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1/6/2020 5:02</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1/6/2020 5:03</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1/6/2020 5:04</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1/6/2020 5:05</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1/6/2020 5:06</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1/6/2020 5:07</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1/6/2020 5:08</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1/6/2020 5:09</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1/6/2020 5:10</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1/6/2020 5:11</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1/6/2020 5:12</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1/6/2020 5:13</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1/6/2020 5:14</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1/6/2020 5:15</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1/6/2020  5:16:50 AM OVER W4 START W5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1/6/2020  5:24:31 AM - PlecareBeliu</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1/6/2020 5:25</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1/6/2020  5:26:33 AM - Tagadau</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1/6/2020 5:27</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1/6/2020 5:28</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1/6/2020 5:29</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1/6/2020 5:30</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1/6/2020 5:31</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1/6/2020 5:32</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1/6/2020 5:33</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1/6/2020 5:34</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1/6/2020  5:35:31 AM - Hasmas</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1/6/2020 5:36</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1/6/2020 5:37</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1/6/2020 5:38</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1/6/2020 5:39</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1/6/2020 5:40</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1/6/2020 5:41</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1/6/2020 5:42</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1/6/2020 5:43</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1/6/2020 5:44</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1/6/2020 5:45</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1/6/2020 5:46</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1/6/2020 5:47</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1/6/2020 5:48</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1/6/2020 5:49</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1/6/2020  5:50:47 AM - SatVacanta</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1/6/2020 5:51</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1/6/2020 5:52</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1/6/2020 5:53</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1/6/2020 5:54</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1/6/2020 5:55</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1/6/2020 5:56</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1/6/2020 5:57</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1/6/2020 5:58</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1/6/2020  5:59:56 AM - Oprire1 Padure</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1/6/2020 6:00</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1/6/2020 6:01</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1/6/2020 6:02</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1/6/2020 6:03</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1/6/2020 6:04</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1/6/2020  6:05:26 AM - Out din Padure</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1/6/2020 6:06</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1/6/2020 6:07</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1/6/2020 6:08</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1/6/2020 6:09</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1/6/2020 6:10</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1/6/2020  6:11:32 AM - Barzesti</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1/6/2020 6:12</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1/6/2020 6:13</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1/6/2020 6:16</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1/6/2020  6:17:38 AM - ResetSenzor</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1/6/2020 6:18</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1/6/2020 6:19</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1/6/2020 6:20</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1/6/2020 6:21</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1/6/2020 6:22</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1/6/2020 6:23</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1/6/2020 6:24</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1/6/2020 6:25</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1/6/2020 6:26</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1/6/2020  6:27:49 AM - Beliu</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1/6/2020 6:28</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1/6/2020 6:29</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1/6/2020 6:30</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1/6/2020 6:31</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1/6/2020 6:32</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1/6/2020 6:33</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1/6/2020 6:34</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1/6/2020 6:35</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1/6/2020 6:36</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1/6/2020 6:37</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1/6/2020 6:39</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1/6/2020 6:40</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1/6/2020 6:41</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1/6/2020 6:42</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1/6/2020 6:43</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1/6/2020 6:44</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1/6/2020  6:45:06 AM AcasaIneu - Terasa</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1/6/2020 6:46</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1/6/2020 6:47</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1/6/2020 6:48</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1/6/2020 6:49</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1/6/2020 6:50</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1/6/2020 6:51</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1/6/2020 6:52</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1/6/2020 6:53</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1/6/2020 6:54</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1/6/2020 6:55</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1/6/2020 6:56</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1/6/2020 6:57</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>W4W5_BeliuGroseniIneu_01_06!$F$2:$F$159</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="158"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="148469632"/>
+        <c:axId val="148471168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="148469632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="148471168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="148471168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="148469632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'W5'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -5365,24 +6392,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84125952"/>
-        <c:axId val="84127744"/>
+        <c:axId val="88351104"/>
+        <c:axId val="88352640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84125952"/>
+        <c:axId val="88351104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84127744"/>
+        <c:crossAx val="88352640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84127744"/>
+        <c:axId val="88352640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1650000.0000000002"/>
@@ -5391,7 +6418,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84125952"/>
+        <c:crossAx val="88351104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5404,7 +6431,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5527,6 +6554,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5857,8 +6914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O159"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection sqref="A1:O66"/>
+    <sheetView tabSelected="1" topLeftCell="O102" workbookViewId="0">
+      <selection activeCell="T136" sqref="T136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13262,7 +14319,7 @@
   <dimension ref="A1:O92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" activeCellId="1" sqref="G1:G1048576 B1:B1048576"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17606,7 +18663,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20725,7 +21782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
07.06 - Done Capitolul 5
To Do - Concluzii
</commit_message>
<xml_diff>
--- a/Documentatie/RezultateExperimentale/W4W5_BeliuGroseniIneu_01_06.xlsx
+++ b/Documentatie/RezultateExperimentale/W4W5_BeliuGroseniIneu_01_06.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="W4W5_BeliuGroseniIneu_01_06" sheetId="1" r:id="rId1"/>
@@ -1647,24 +1647,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87510016"/>
-        <c:axId val="87581440"/>
+        <c:axId val="115943296"/>
+        <c:axId val="115944832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87510016"/>
+        <c:axId val="115943296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87581440"/>
+        <c:crossAx val="115944832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87581440"/>
+        <c:axId val="115944832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1672,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87510016"/>
+        <c:crossAx val="115943296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1685,7 +1685,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2674,24 +2674,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87723392"/>
-        <c:axId val="87943040"/>
+        <c:axId val="115953024"/>
+        <c:axId val="115983488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87723392"/>
+        <c:axId val="115953024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87943040"/>
+        <c:crossAx val="115983488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87943040"/>
+        <c:axId val="115983488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2699,7 +2699,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87723392"/>
+        <c:crossAx val="115953024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2712,7 +2712,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3701,24 +3701,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88013056"/>
-        <c:axId val="88031232"/>
+        <c:axId val="116220672"/>
+        <c:axId val="116222208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88013056"/>
+        <c:axId val="116220672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="t"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88031232"/>
+        <c:crossAx val="116222208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88031232"/>
+        <c:axId val="116222208"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3726,7 +3726,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88013056"/>
+        <c:crossAx val="116220672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3739,7 +3739,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4728,24 +4728,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88085248"/>
-        <c:axId val="88086784"/>
+        <c:axId val="116230016"/>
+        <c:axId val="116231552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88085248"/>
+        <c:axId val="116230016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88086784"/>
+        <c:crossAx val="116231552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88086784"/>
+        <c:axId val="116231552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4753,7 +4753,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88085248"/>
+        <c:crossAx val="116230016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4766,7 +4766,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5755,24 +5755,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="148469632"/>
-        <c:axId val="148471168"/>
+        <c:axId val="116612096"/>
+        <c:axId val="116634368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="148469632"/>
+        <c:axId val="116612096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148471168"/>
+        <c:crossAx val="116634368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148471168"/>
+        <c:axId val="116634368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5780,7 +5780,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148469632"/>
+        <c:crossAx val="116612096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5793,7 +5793,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6392,24 +6392,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="88351104"/>
-        <c:axId val="88352640"/>
+        <c:axId val="116688384"/>
+        <c:axId val="116689920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88351104"/>
+        <c:axId val="116688384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88352640"/>
+        <c:crossAx val="116689920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88352640"/>
+        <c:axId val="116689920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1650000.0000000002"/>
@@ -6418,7 +6418,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88351104"/>
+        <c:crossAx val="116688384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6431,7 +6431,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6914,7 +6914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O102" workbookViewId="0">
+    <sheetView topLeftCell="H3" workbookViewId="0">
       <selection activeCell="T136" sqref="T136"/>
     </sheetView>
   </sheetViews>
@@ -18662,8 +18662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
11.06 Inscriere + Corectat
</commit_message>
<xml_diff>
--- a/Documentatie/RezultateExperimentale/W4W5_BeliuGroseniIneu_01_06.xlsx
+++ b/Documentatie/RezultateExperimentale/W4W5_BeliuGroseniIneu_01_06.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="W4W5_BeliuGroseniIneu_01_06" sheetId="1" r:id="rId1"/>
     <sheet name="W5" sheetId="2" r:id="rId2"/>
     <sheet name="W4" sheetId="3" r:id="rId3"/>
     <sheet name="Formule" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="35">
   <si>
     <t>Device</t>
   </si>
@@ -1647,24 +1648,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115943296"/>
-        <c:axId val="115944832"/>
+        <c:axId val="121579392"/>
+        <c:axId val="121580928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115943296"/>
+        <c:axId val="121579392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115944832"/>
+        <c:crossAx val="121580928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115944832"/>
+        <c:axId val="121580928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,7 +1673,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115943296"/>
+        <c:crossAx val="121579392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1685,7 +1686,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2674,24 +2675,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="115953024"/>
-        <c:axId val="115983488"/>
+        <c:axId val="121589120"/>
+        <c:axId val="121619584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115953024"/>
+        <c:axId val="121589120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115983488"/>
+        <c:crossAx val="121619584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115983488"/>
+        <c:axId val="121619584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2699,7 +2700,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115953024"/>
+        <c:crossAx val="121589120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2712,7 +2713,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2722,9 +2723,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -3701,24 +3700,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="116220672"/>
-        <c:axId val="116222208"/>
+        <c:axId val="121983744"/>
+        <c:axId val="121985280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116220672"/>
+        <c:axId val="121983744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="t"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116222208"/>
+        <c:crossAx val="121985280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116222208"/>
+        <c:axId val="121985280"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3726,20 +3725,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116220672"/>
+        <c:crossAx val="121983744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3749,9 +3747,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -4728,24 +4724,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="116230016"/>
-        <c:axId val="116231552"/>
+        <c:axId val="121993088"/>
+        <c:axId val="121994624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116230016"/>
+        <c:axId val="121993088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116231552"/>
+        <c:crossAx val="121994624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116231552"/>
+        <c:axId val="121994624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4753,20 +4749,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116230016"/>
+        <c:crossAx val="121993088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4776,9 +4771,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -5755,24 +5748,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="116612096"/>
-        <c:axId val="116634368"/>
+        <c:axId val="122182656"/>
+        <c:axId val="122204928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116612096"/>
+        <c:axId val="122182656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116634368"/>
+        <c:crossAx val="122204928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116634368"/>
+        <c:axId val="122204928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5780,20 +5773,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116612096"/>
+        <c:crossAx val="122182656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5803,9 +5795,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -6392,24 +6382,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="116688384"/>
-        <c:axId val="116689920"/>
+        <c:axId val="122258944"/>
+        <c:axId val="122260480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116688384"/>
+        <c:axId val="122258944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116689920"/>
+        <c:crossAx val="122260480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116689920"/>
+        <c:axId val="122260480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1650000.0000000002"/>
@@ -6418,20 +6408,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116688384"/>
+        <c:crossAx val="122258944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6914,8 +6903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O159"/>
   <sheetViews>
-    <sheetView topLeftCell="H3" workbookViewId="0">
-      <selection activeCell="T136" sqref="T136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14318,8 +14307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18662,7 +18651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -21790,4 +21779,404 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="6" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43836.245011574072</v>
+      </c>
+      <c r="C2">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>83</v>
+      </c>
+      <c r="E2">
+        <v>137</v>
+      </c>
+      <c r="F2">
+        <v>33</v>
+      </c>
+      <c r="G2">
+        <v>1695233</v>
+      </c>
+      <c r="H2">
+        <v>5627469</v>
+      </c>
+      <c r="I2">
+        <v>1684771</v>
+      </c>
+      <c r="J2">
+        <v>5626695</v>
+      </c>
+      <c r="K2">
+        <v>137</v>
+      </c>
+      <c r="L2">
+        <v>25.8</v>
+      </c>
+      <c r="M2">
+        <v>43.66</v>
+      </c>
+      <c r="N2">
+        <v>989.17</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43836.245717592596</v>
+      </c>
+      <c r="C3">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>72</v>
+      </c>
+      <c r="E3">
+        <v>105</v>
+      </c>
+      <c r="F3">
+        <v>41</v>
+      </c>
+      <c r="G3">
+        <v>1694385</v>
+      </c>
+      <c r="H3">
+        <v>5627696</v>
+      </c>
+      <c r="I3">
+        <v>1681627</v>
+      </c>
+      <c r="J3">
+        <v>5626107</v>
+      </c>
+      <c r="K3">
+        <v>105</v>
+      </c>
+      <c r="L3">
+        <v>25.8</v>
+      </c>
+      <c r="M3">
+        <v>43.66</v>
+      </c>
+      <c r="N3">
+        <v>989.17</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2">
+        <v>43836.246423611112</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>71</v>
+      </c>
+      <c r="E4">
+        <v>107</v>
+      </c>
+      <c r="F4">
+        <v>39</v>
+      </c>
+      <c r="G4">
+        <v>1693278</v>
+      </c>
+      <c r="H4">
+        <v>5627709</v>
+      </c>
+      <c r="I4">
+        <v>1681834</v>
+      </c>
+      <c r="J4">
+        <v>5626311</v>
+      </c>
+      <c r="K4">
+        <v>107</v>
+      </c>
+      <c r="L4">
+        <v>25.8</v>
+      </c>
+      <c r="M4">
+        <v>43.66</v>
+      </c>
+      <c r="N4">
+        <v>989.17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43836.247129629628</v>
+      </c>
+      <c r="C5">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>79</v>
+      </c>
+      <c r="E5">
+        <v>106</v>
+      </c>
+      <c r="F5">
+        <v>37</v>
+      </c>
+      <c r="G5">
+        <v>1692743</v>
+      </c>
+      <c r="H5">
+        <v>5627555</v>
+      </c>
+      <c r="I5">
+        <v>1681669</v>
+      </c>
+      <c r="J5">
+        <v>5626424</v>
+      </c>
+      <c r="K5">
+        <v>106</v>
+      </c>
+      <c r="L5">
+        <v>24.26</v>
+      </c>
+      <c r="M5">
+        <v>45.25</v>
+      </c>
+      <c r="N5">
+        <v>983.05</v>
+      </c>
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2">
+        <v>43836.247835648152</v>
+      </c>
+      <c r="C6">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>79</v>
+      </c>
+      <c r="E6">
+        <v>106</v>
+      </c>
+      <c r="F6">
+        <v>37</v>
+      </c>
+      <c r="G6">
+        <v>1692743</v>
+      </c>
+      <c r="H6">
+        <v>5627555</v>
+      </c>
+      <c r="I6">
+        <v>1681669</v>
+      </c>
+      <c r="J6">
+        <v>5626424</v>
+      </c>
+      <c r="K6">
+        <v>106</v>
+      </c>
+      <c r="L6">
+        <v>24.26</v>
+      </c>
+      <c r="M6">
+        <v>45.25</v>
+      </c>
+      <c r="N6">
+        <v>983.05</v>
+      </c>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43836.248541666668</v>
+      </c>
+      <c r="C7">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>70</v>
+      </c>
+      <c r="E7">
+        <v>98</v>
+      </c>
+      <c r="F7">
+        <v>38</v>
+      </c>
+      <c r="G7">
+        <v>1692558</v>
+      </c>
+      <c r="H7">
+        <v>5627730</v>
+      </c>
+      <c r="I7">
+        <v>1681122</v>
+      </c>
+      <c r="J7">
+        <v>5626379</v>
+      </c>
+      <c r="K7">
+        <v>98</v>
+      </c>
+      <c r="L7">
+        <v>24.26</v>
+      </c>
+      <c r="M7">
+        <v>45.25</v>
+      </c>
+      <c r="N7">
+        <v>983.05</v>
+      </c>
+      <c r="O7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43836.249247685184</v>
+      </c>
+      <c r="C8">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>74</v>
+      </c>
+      <c r="E8">
+        <v>88</v>
+      </c>
+      <c r="F8">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>1692270</v>
+      </c>
+      <c r="H8">
+        <v>5627653</v>
+      </c>
+      <c r="I8">
+        <v>1680764</v>
+      </c>
+      <c r="J8">
+        <v>5626132</v>
+      </c>
+      <c r="K8">
+        <v>88</v>
+      </c>
+      <c r="L8">
+        <v>24.26</v>
+      </c>
+      <c r="M8">
+        <v>45.25</v>
+      </c>
+      <c r="N8">
+        <v>983.05</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>